<commit_message>
Create Deposit and Withdrawal actions
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos Oliveira\source\repos\ATM-Machine\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DC1194-43F2-42FF-AA4C-F334227C7354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334A1F9E-1918-4DC7-AA76-D9040C6FB3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>userId</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Oliveira</t>
+  </si>
+  <si>
+    <t>Elisa</t>
   </si>
 </sst>
 </file>
@@ -95,9 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,7 +385,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +423,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -440,11 +444,38 @@
         <v>2500</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>111111</v>
+      </c>
+      <c r="E3">
+        <v>20598</v>
+      </c>
+      <c r="F3">
+        <v>5995</v>
+      </c>
+      <c r="G3">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="1"/>
+      <c r="G14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>